<commit_message>
updating the excel sheet and adding the associated notebook
</commit_message>
<xml_diff>
--- a/HPE_NVDA_datagen.xlsx
+++ b/HPE_NVDA_datagen.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20416"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\corp.nsa.ic.gov\udroot$\gh1\vol20354\eagelbe\private\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eagelbe\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68676E76-5D6A-4B3E-A04A-815C727E7E7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{545B395C-63EE-4D64-B310-E501B0487BD6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="31635" windowHeight="13725" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data_sources" sheetId="1" r:id="rId1"/>
     <sheet name="joins" sheetId="2" r:id="rId2"/>
-    <sheet name="table_a" sheetId="7" r:id="rId3"/>
-    <sheet name="table_b" sheetId="3" r:id="rId4"/>
-    <sheet name="table_c" sheetId="4" r:id="rId5"/>
-    <sheet name="table_d" sheetId="5" r:id="rId6"/>
-    <sheet name="table_e" sheetId="6" r:id="rId7"/>
+    <sheet name="all_joins" sheetId="9" r:id="rId3"/>
+    <sheet name="table_a" sheetId="7" r:id="rId4"/>
+    <sheet name="table_b" sheetId="3" r:id="rId5"/>
+    <sheet name="table_c" sheetId="4" r:id="rId6"/>
+    <sheet name="table_d" sheetId="5" r:id="rId7"/>
+    <sheet name="table_e" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="91">
   <si>
     <t>masked_table_id</t>
   </si>
@@ -96,9 +97,6 @@
     <t>col_c_10</t>
   </si>
   <si>
-    <t>column_name</t>
-  </si>
-  <si>
     <t>spark_data_type</t>
   </si>
   <si>
@@ -295,6 +293,18 @@
   </si>
   <si>
     <t>col_e_8</t>
+  </si>
+  <si>
+    <t>cannot be joined at the same time as the join in row 13</t>
+  </si>
+  <si>
+    <t>cannot be joined at the same time as the join in row 12</t>
+  </si>
+  <si>
+    <t>cannot be joined at the same time as the join in row 11</t>
+  </si>
+  <si>
+    <t>cannot be joined at the same time as the join in row 14</t>
   </si>
 </sst>
 </file>
@@ -694,8 +704,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,7 +776,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -902,11 +912,287 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB3089E2-3FA4-4296-957A-DECDDDB6B328}">
+  <dimension ref="A1:F14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="8.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5703125" style="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="20" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" s="20" t="s">
+        <v>87</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -919,24 +1205,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>25</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>26</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="10"/>
@@ -946,7 +1232,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="9">
         <v>0</v>
@@ -957,10 +1243,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9">
         <v>0</v>
@@ -971,10 +1257,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>30</v>
       </c>
       <c r="C5" s="9">
         <v>-1</v>
@@ -985,10 +1271,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>32</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="10"/>
@@ -998,7 +1284,7 @@
         <v>18</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="9">
         <v>0</v>
@@ -1009,10 +1295,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="9">
         <v>-1</v>
@@ -1023,10 +1309,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C9" s="9">
         <v>0</v>
@@ -1037,20 +1323,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="9">
         <v>-1</v>
@@ -1061,10 +1347,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="9">
         <v>-100</v>
@@ -1075,10 +1361,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="9">
         <v>17000000000</v>
@@ -1089,10 +1375,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="9">
         <v>0</v>
@@ -1103,10 +1389,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="9">
         <v>0</v>
@@ -1132,7 +1418,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
@@ -1150,43 +1436,43 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="D1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="D2" s="23"/>
       <c r="E2" s="23"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>46</v>
       </c>
       <c r="D3" s="23">
         <v>5</v>
@@ -1197,26 +1483,26 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="23"/>
       <c r="E4" s="23"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D5" s="23">
         <v>2</v>
@@ -1227,13 +1513,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>49</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>50</v>
       </c>
       <c r="D6" s="23">
         <v>32</v>
@@ -1244,52 +1530,52 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D8" s="23"/>
       <c r="E8" s="23"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="24">
         <v>16843009</v>
@@ -1300,13 +1586,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="24">
         <v>37263149</v>
@@ -1317,13 +1603,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="24">
         <v>100</v>
@@ -1334,13 +1620,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" s="24">
         <v>1600000000</v>
@@ -1351,13 +1637,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D14" s="24">
         <v>1600000000</v>
@@ -1368,13 +1654,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
@@ -1384,11 +1670,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1403,74 +1689,74 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="D1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" s="26" t="s">
+      <c r="E1" s="26" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="26" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B4" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="26">
         <v>1</v>
@@ -1481,13 +1767,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D7" s="26">
         <v>1</v>
@@ -1498,24 +1784,24 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B9" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="24">
         <v>1600000000</v>
@@ -1526,13 +1812,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D10" s="24">
         <v>1600000000</v>
@@ -1546,10 +1832,10 @@
         <v>19</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" s="27">
         <v>16777217</v>
@@ -1563,10 +1849,10 @@
         <v>20</v>
       </c>
       <c r="B12" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D12" s="27">
         <v>16777217</v>
@@ -1577,13 +1863,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B13" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D13" s="26">
         <v>-1</v>
@@ -1594,13 +1880,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1608,12 +1894,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,19 +1912,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1646,30 +1932,30 @@
         <v>15</v>
       </c>
       <c r="B2" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="21">
+        <v>0</v>
+      </c>
+      <c r="E2" s="21">
         <v>9.2233720368547697E+18</v>
-      </c>
-      <c r="E2" s="21">
-        <v>3.1750376728716902E+18</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3" s="21">
-        <v>2.1617278211378301E+17</v>
+        <v>0</v>
       </c>
       <c r="E3" s="21">
         <v>9.2233720368547697E+18</v>
@@ -1677,35 +1963,35 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D6" s="21">
         <v>1</v>
@@ -1716,48 +2002,52 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>44</v>
-      </c>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1771,19 +2061,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="D1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>23</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,10 +2081,10 @@
         <v>16</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D2" s="21">
         <v>16778241</v>
@@ -1805,35 +2095,35 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="20" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" s="21">
         <v>0</v>
@@ -1844,57 +2134,57 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B7" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="B7" s="21" t="s">
-        <v>84</v>
-      </c>
       <c r="C7" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>